<commit_message>
No Gambar, Fix Report, Delete Exel
</commit_message>
<xml_diff>
--- a/backend/public/excel/order.xlsx
+++ b/backend/public/excel/order.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>No</t>
   </si>
@@ -41,42 +41,6 @@
   </si>
   <si>
     <t>Total Price</t>
-  </si>
-  <si>
-    <t>ORD-1734751268058</t>
-  </si>
-  <si>
-    <t>120.000</t>
-  </si>
-  <si>
-    <t>13.200</t>
-  </si>
-  <si>
-    <t>133.200</t>
-  </si>
-  <si>
-    <t>Sample Product</t>
-  </si>
-  <si>
-    <t>25.000</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>50.000</t>
-  </si>
-  <si>
-    <t>ORD-1734965883273</t>
-  </si>
-  <si>
-    <t>2.750</t>
-  </si>
-  <si>
-    <t>27.750</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
 </sst>
 </file>
@@ -122,11 +86,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
@@ -512,70 +474,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
-        <v>45645.15791666666</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
-        <v>45649.62364583333</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>